<commit_message>
Generic Utilities Implementation in test scripts
</commit_message>
<xml_diff>
--- a/src/test/resources/VtigerCRMTestData.xlsx
+++ b/src/test/resources/VtigerCRMTestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20375"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QPS-Basavanagudi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sncsr\git\QSPGL-JSP-101\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A1997E0-ABA5-4792-8B21-1F6C82EABC5E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C91602-8FB2-45F3-B4EA-79CD84304EBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" xr2:uid="{A6492B4B-4497-484C-9067-5A512381FFD5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A6492B4B-4497-484C-9067-5A512381FFD5}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
@@ -610,7 +610,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>